<commit_message>
initial place url rather than reviews url
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/stajdini_iu_edu/Documents/Research/python scripts/googlemaps-scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC1048D6191F70B45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B65172D-9E4F-426F-887E-785324C3E230}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="11_F25DC773A252ABDACC1048D6191F70B45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{339E22E7-717D-4C07-A4A1-DA233516CAAC}"/>
   <bookViews>
     <workbookView xWindow="1098" yWindow="258" windowWidth="14682" windowHeight="12246" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>https://www.google.it/maps/place/Pantheon/@41.8986108,12.4746842,17z/data=!3m1!4b1!4m7!3m6!1s0x132f604f678640a9:0xcad165fa2036ce2c!8m2!3d41.8986108!4d12.4768729!9m1!1b1</t>
+    <t>https://www.google.it/maps/place/Pantheon/@41.8986108,12.4768729,17z/data=!4m16!1m9!3m8!1s0x132f604f678640a9:0xcad165fa2036ce2c!2sPantheon!8m2!3d41.8986108!4d12.4768729!9m1!1b1!16zL20vMDF4emR6!3m5!1s0x132f604f678640a9:0xcad165fa2036ce2c!8m2!3d41.8986108!4d12.4768729!16zL20vMDF4emR6?entry=ttu</t>
+  </si>
+  <si>
+    <t>https://www.google.it/maps/place/Giolitti/@41.8986032,12.4765859,16.72z/data=!3m1!5s0x132f60519c07e5ef:0x2f3920985ad7eae7!4m16!1m9!3m8!1s0x132f604f678640a9:0xcad165fa2036ce2c!2sPantheon!8m2!3d41.8986108!4d12.4768729!9m1!1b1!16zL20vMDF4emR6!3m5!1s0x132f60519cfa737b:0x38610a40a28f8107!8m2!3d41.9011019!4d12.4771847!16zL20vMGMwMzBu?entry=ttu</t>
   </si>
 </sst>
 </file>
@@ -356,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -369,7 +372,15 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.google.it/maps/place/Pantheon/@41.8986108,12.4768729,17z/data=!4m16!1m9!3m8!1s0x132f604f678640a9:0xcad165fa2036ce2c!2sPantheon!8m2!3d41.8986108!4d12.4768729!9m1!1b1!16zL20vMDF4emR6!3m5!1s0x132f604f678640a9:0xcad165fa2036ce2c!8m2!3d41.8986108!4d12.4768729!16zL20vMDF4emR6?entry=ttu" xr:uid="{6118E87D-6D1E-47A6-935C-6AAF41296950}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>